<commit_message>
Change All Folder to Files folder
</commit_message>
<xml_diff>
--- a/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
+++ b/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
@@ -748,6 +748,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -756,54 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,32 +1400,32 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93" t="s">
+      <c r="D4" s="90"/>
+      <c r="E4" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="94"/>
-      <c r="G4" s="93" t="s">
+      <c r="F4" s="92"/>
+      <c r="G4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="94"/>
-      <c r="I4" s="93" t="s">
+      <c r="H4" s="92"/>
+      <c r="I4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="87" t="s">
+      <c r="J4" s="92"/>
+      <c r="K4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="85" t="s">
+      <c r="L4" s="83" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="41"/>
@@ -1444,8 +1444,8 @@
       <c r="R4" s="35"/>
     </row>
     <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="86"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
@@ -1470,8 +1470,8 @@
       <c r="J5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="88"/>
-      <c r="L5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="84"/>
       <c r="M5" s="41"/>
       <c r="N5" s="33">
         <v>41152</v>
@@ -2141,10 +2141,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="84"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="58">
         <f t="shared" ref="C19:J19" si="12">SUM(C6:C18)</f>
         <v>11420</v>
@@ -2372,132 +2372,147 @@
       <c r="F34" s="37"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="78"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="79" t="s">
+      <c r="E35" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="79"/>
+      <c r="F35" s="95"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="80" t="s">
+      <c r="B36" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="81"/>
+      <c r="C36" s="78"/>
       <c r="D36" s="65">
         <f>J20</f>
         <v>0</v>
       </c>
-      <c r="E36" s="82" t="s">
+      <c r="E36" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="83"/>
+      <c r="F36" s="80"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="81"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="65">
         <f>R20</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E37" s="82" t="s">
+      <c r="E37" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="83"/>
+      <c r="F37" s="80"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="81"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="65">
         <f>+D36+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E38" s="82" t="s">
+      <c r="E38" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="83"/>
+      <c r="F38" s="80"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="80" t="s">
+      <c r="B39" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="81"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="65">
         <f>'Bang tra no'!C11</f>
         <v>0</v>
       </c>
-      <c r="E39" s="82" t="s">
+      <c r="E39" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="83"/>
+      <c r="F39" s="80"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="81"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="65">
         <f>D39+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E40" s="82" t="s">
+      <c r="E40" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="83"/>
+      <c r="F40" s="80"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="81"/>
+      <c r="C41" s="78"/>
       <c r="D41" s="65">
         <f>D40/2</f>
         <v>9154036.6301369853</v>
       </c>
-      <c r="E41" s="82" t="s">
+      <c r="E41" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="83"/>
+      <c r="F41" s="80"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="81"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="65">
         <f>'Bang tra no'!F11</f>
         <v>131877073.26027396</v>
       </c>
-      <c r="E42" s="82" t="s">
+      <c r="E42" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="83"/>
+      <c r="F42" s="80"/>
     </row>
     <row r="43" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="95" t="s">
+      <c r="B43" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="81"/>
+      <c r="C43" s="78"/>
       <c r="D43" s="65">
         <f>D42-D41</f>
         <v>122723036.63013698</v>
       </c>
-      <c r="E43" s="82" t="s">
+      <c r="E43" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="83"/>
+      <c r="F43" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="B42:C42"/>
@@ -2510,21 +2525,6 @@
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit prototype of AnhLT
</commit_message>
<xml_diff>
--- a/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
+++ b/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="765" windowWidth="15570" windowHeight="6705" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="765" windowWidth="15570" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Du no TD" sheetId="3" r:id="rId1"/>
@@ -748,6 +748,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -756,54 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1400,32 +1400,32 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93" t="s">
+      <c r="D4" s="90"/>
+      <c r="E4" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="94"/>
-      <c r="G4" s="93" t="s">
+      <c r="F4" s="92"/>
+      <c r="G4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="94"/>
-      <c r="I4" s="93" t="s">
+      <c r="H4" s="92"/>
+      <c r="I4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="87" t="s">
+      <c r="J4" s="92"/>
+      <c r="K4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="85" t="s">
+      <c r="L4" s="83" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="41"/>
@@ -1444,8 +1444,8 @@
       <c r="R4" s="35"/>
     </row>
     <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="86"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
@@ -1470,8 +1470,8 @@
       <c r="J5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="88"/>
-      <c r="L5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="84"/>
       <c r="M5" s="41"/>
       <c r="N5" s="33">
         <v>41152</v>
@@ -2141,10 +2141,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="84"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="58">
         <f t="shared" ref="C19:J19" si="12">SUM(C6:C18)</f>
         <v>11420</v>
@@ -2372,132 +2372,147 @@
       <c r="F34" s="37"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="78"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="79" t="s">
+      <c r="E35" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="79"/>
+      <c r="F35" s="95"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="80" t="s">
+      <c r="B36" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="81"/>
+      <c r="C36" s="78"/>
       <c r="D36" s="65">
         <f>J20</f>
         <v>0</v>
       </c>
-      <c r="E36" s="82" t="s">
+      <c r="E36" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="83"/>
+      <c r="F36" s="80"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="81"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="65">
         <f>R20</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E37" s="82" t="s">
+      <c r="E37" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="83"/>
+      <c r="F37" s="80"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="81"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="65">
         <f>+D36+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E38" s="82" t="s">
+      <c r="E38" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="83"/>
+      <c r="F38" s="80"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="80" t="s">
+      <c r="B39" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="81"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="65">
         <f>'Bang tra no'!C11</f>
         <v>0</v>
       </c>
-      <c r="E39" s="82" t="s">
+      <c r="E39" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="83"/>
+      <c r="F39" s="80"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="81"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="65">
         <f>D39+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E40" s="82" t="s">
+      <c r="E40" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="83"/>
+      <c r="F40" s="80"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="81"/>
+      <c r="C41" s="78"/>
       <c r="D41" s="65">
         <f>D40/2</f>
         <v>9154036.6301369853</v>
       </c>
-      <c r="E41" s="82" t="s">
+      <c r="E41" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="83"/>
+      <c r="F41" s="80"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="81"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="65">
         <f>'Bang tra no'!F11</f>
         <v>131877073.26027396</v>
       </c>
-      <c r="E42" s="82" t="s">
+      <c r="E42" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="83"/>
+      <c r="F42" s="80"/>
     </row>
     <row r="43" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="95" t="s">
+      <c r="B43" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="81"/>
+      <c r="C43" s="78"/>
       <c r="D43" s="65">
         <f>D42-D41</f>
         <v>122723036.63013698</v>
       </c>
-      <c r="E43" s="82" t="s">
+      <c r="E43" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="83"/>
+      <c r="F43" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="B42:C42"/>
@@ -2510,21 +2525,6 @@
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2538,7 +2538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Delete old use case ! commit code
</commit_message>
<xml_diff>
--- a/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
+++ b/document/Files/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="765" windowWidth="15570" windowHeight="6705"/>
+    <workbookView xWindow="120" yWindow="765" windowWidth="15570" windowHeight="6705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Du no TD" sheetId="3" r:id="rId1"/>
@@ -748,6 +748,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -760,50 +769,41 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1400,32 +1400,32 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91" t="s">
+      <c r="D4" s="92"/>
+      <c r="E4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="91" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="92"/>
-      <c r="I4" s="91" t="s">
+      <c r="H4" s="94"/>
+      <c r="I4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="85" t="s">
+      <c r="J4" s="94"/>
+      <c r="K4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="83" t="s">
+      <c r="L4" s="85" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="41"/>
@@ -1444,8 +1444,8 @@
       <c r="R4" s="35"/>
     </row>
     <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="84"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
@@ -1470,8 +1470,8 @@
       <c r="J5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="84"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="86"/>
       <c r="M5" s="41"/>
       <c r="N5" s="33">
         <v>41152</v>
@@ -2141,10 +2141,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="82"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="58">
         <f t="shared" ref="C19:J19" si="12">SUM(C6:C18)</f>
         <v>11420</v>
@@ -2372,147 +2372,132 @@
       <c r="F34" s="37"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="94"/>
+      <c r="C35" s="78"/>
       <c r="D35" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="95" t="s">
+      <c r="E35" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="95"/>
+      <c r="F35" s="79"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="77" t="s">
+      <c r="B36" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="78"/>
+      <c r="C36" s="81"/>
       <c r="D36" s="65">
         <f>J20</f>
         <v>0</v>
       </c>
-      <c r="E36" s="79" t="s">
+      <c r="E36" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="80"/>
+      <c r="F36" s="83"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="78"/>
+      <c r="C37" s="81"/>
       <c r="D37" s="65">
         <f>R20</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E37" s="79" t="s">
+      <c r="E37" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="80"/>
+      <c r="F37" s="83"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="77" t="s">
+      <c r="B38" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="78"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="65">
         <f>+D36+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E38" s="79" t="s">
+      <c r="E38" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="80"/>
+      <c r="F38" s="83"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="78"/>
+      <c r="C39" s="81"/>
       <c r="D39" s="65">
         <f>'Bang tra no'!C11</f>
         <v>0</v>
       </c>
-      <c r="E39" s="79" t="s">
+      <c r="E39" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="80"/>
+      <c r="F39" s="83"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="77" t="s">
+      <c r="B40" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="78"/>
+      <c r="C40" s="81"/>
       <c r="D40" s="65">
         <f>D39+D37</f>
         <v>18308073.260273971</v>
       </c>
-      <c r="E40" s="79" t="s">
+      <c r="E40" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="80"/>
+      <c r="F40" s="83"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="77" t="s">
+      <c r="B41" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="78"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="65">
         <f>D40/2</f>
         <v>9154036.6301369853</v>
       </c>
-      <c r="E41" s="79" t="s">
+      <c r="E41" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="80"/>
+      <c r="F41" s="83"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="77" t="s">
+      <c r="B42" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="78"/>
+      <c r="C42" s="81"/>
       <c r="D42" s="65">
         <f>'Bang tra no'!F11</f>
         <v>131877073.26027396</v>
       </c>
-      <c r="E42" s="79" t="s">
+      <c r="E42" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="80"/>
+      <c r="F42" s="83"/>
     </row>
     <row r="43" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="81" t="s">
+      <c r="B43" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="78"/>
+      <c r="C43" s="81"/>
       <c r="D43" s="65">
         <f>D42-D41</f>
         <v>122723036.63013698</v>
       </c>
-      <c r="E43" s="79" t="s">
+      <c r="E43" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="80"/>
+      <c r="F43" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="B42:C42"/>
@@ -2525,6 +2510,21 @@
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="E41:F41"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2538,7 +2538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>

</xml_diff>